<commit_message>
update downstream count data with 2023 results
</commit_message>
<xml_diff>
--- a/1. data/downstream_smolt_data.xlsx
+++ b/1. data/downstream_smolt_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\Barkley-Sk-CSAS\1. data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5204AA3-E670-4A6A-9A7B-F2DA753C0615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36DF478-B9BE-4188-B416-134FCD4E0399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8C1C5B83-4466-4FD1-9733-C3409F81B779}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8C1C5B83-4466-4FD1-9733-C3409F81B779}"/>
   </bookViews>
   <sheets>
     <sheet name="Hucuktlis" sheetId="1" r:id="rId1"/>
@@ -446,15 +446,15 @@
       <selection activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>38086</v>
       </c>
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>38087</v>
       </c>
@@ -493,7 +493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>38088</v>
       </c>
@@ -504,7 +504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>38089</v>
       </c>
@@ -515,17 +515,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>38090</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>38091</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>38092</v>
       </c>
@@ -536,7 +536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>38093</v>
       </c>
@@ -547,7 +547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>38094</v>
       </c>
@@ -558,7 +558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>38095</v>
       </c>
@@ -569,17 +569,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>38096</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>38097</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>38098</v>
       </c>
@@ -590,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>38099</v>
       </c>
@@ -601,7 +601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>38100</v>
       </c>
@@ -612,7 +612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>38101</v>
       </c>
@@ -623,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>38102</v>
       </c>
@@ -634,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>38103</v>
       </c>
@@ -645,7 +645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>38104</v>
       </c>
@@ -656,22 +656,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>38105</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>38106</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>38107</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>38108</v>
       </c>
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>38109</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>38110</v>
       </c>
@@ -704,7 +704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>38111</v>
       </c>
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>38112</v>
       </c>
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>38113</v>
       </c>
@@ -734,7 +734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>38114</v>
       </c>
@@ -742,7 +742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>38115</v>
       </c>
@@ -753,7 +753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>38116</v>
       </c>
@@ -764,7 +764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>38117</v>
       </c>
@@ -775,7 +775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>38118</v>
       </c>
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>38119</v>
       </c>
@@ -794,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>38120</v>
       </c>
@@ -805,7 +805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>38121</v>
       </c>
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>38122</v>
       </c>
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38123</v>
       </c>
@@ -838,7 +838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38124</v>
       </c>
@@ -849,12 +849,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>38125</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>38126</v>
       </c>
@@ -865,7 +865,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>38428</v>
       </c>
@@ -874,7 +874,7 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>38429</v>
       </c>
@@ -883,7 +883,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>38430</v>
       </c>
@@ -892,7 +892,7 @@
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>38431</v>
       </c>
@@ -901,7 +901,7 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>38432</v>
       </c>
@@ -910,7 +910,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>38433</v>
       </c>
@@ -919,7 +919,7 @@
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>38434</v>
       </c>
@@ -930,7 +930,7 @@
       </c>
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>38436</v>
       </c>
@@ -941,7 +941,7 @@
       </c>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>38438</v>
       </c>
@@ -952,7 +952,7 @@
       </c>
       <c r="E51" s="2"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>38440</v>
       </c>
@@ -965,7 +965,7 @@
       </c>
       <c r="E52" s="2"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>38443</v>
       </c>
@@ -978,7 +978,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>38445</v>
       </c>
@@ -989,7 +989,7 @@
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>38446</v>
       </c>
@@ -1000,7 +1000,7 @@
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>38450</v>
       </c>
@@ -1011,7 +1011,7 @@
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>38451</v>
       </c>
@@ -1024,7 +1024,7 @@
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>38452</v>
       </c>
@@ -1037,7 +1037,7 @@
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>38453</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>38465</v>
       </c>
@@ -1061,7 +1061,7 @@
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>38467</v>
       </c>
@@ -1074,7 +1074,7 @@
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>38468</v>
       </c>
@@ -1087,7 +1087,7 @@
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>38469</v>
       </c>
@@ -1100,7 +1100,7 @@
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>38470</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>38471</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>38472</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>38474</v>
       </c>
@@ -1154,7 +1154,7 @@
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>38475</v>
       </c>
@@ -1167,7 +1167,7 @@
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>38476</v>
       </c>
@@ -1180,7 +1180,7 @@
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>38478</v>
       </c>
@@ -1193,7 +1193,7 @@
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>38480</v>
       </c>
@@ -1206,7 +1206,7 @@
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>38482</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>38484</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>38486</v>
       </c>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>38487</v>
       </c>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>38491</v>
       </c>
@@ -1272,7 +1272,7 @@
       <c r="E76" s="2"/>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>38492</v>
       </c>
@@ -1284,7 +1284,7 @@
       <c r="E77" s="2"/>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>38497</v>
       </c>
@@ -1296,7 +1296,7 @@
       <c r="E78" s="2"/>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>38498</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="E79" s="2"/>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>38499</v>
       </c>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>38501</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="E81" s="2"/>
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>38502</v>
       </c>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>38503</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="E83" s="2"/>
       <c r="G83" s="1"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>38504</v>
       </c>
@@ -1378,7 +1378,7 @@
       <c r="E84" s="2"/>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>38507</v>
       </c>
@@ -1392,7 +1392,7 @@
       <c r="E85" s="2"/>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>38509</v>
       </c>
@@ -1408,7 +1408,7 @@
       <c r="E86" s="2"/>
       <c r="G86" s="1"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>38511</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="E87" s="2"/>
       <c r="G87" s="1"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>38513</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="E88" s="2"/>
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>38515</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="E89" s="2"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>38516</v>
       </c>
@@ -1465,18 +1465,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4631003-9268-4649-9D95-33D47A827CA5}">
-  <dimension ref="A1:O78"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="8.88671875" style="7"/>
+    <col min="1" max="9" width="8.85546875" style="7"/>
+    <col min="10" max="10" width="9.140625" style="7"/>
+    <col min="11" max="16" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -1505,25 +1507,28 @@
         <v>2024</v>
       </c>
       <c r="J1" s="5">
+        <v>2023</v>
+      </c>
+      <c r="K1" s="5">
         <v>2022</v>
       </c>
-      <c r="K1" s="5">
+      <c r="L1" s="5">
         <v>2021</v>
       </c>
-      <c r="L1" s="5">
+      <c r="M1" s="5">
         <v>2020</v>
       </c>
-      <c r="M1" s="5">
+      <c r="N1" s="5">
         <v>2019</v>
       </c>
-      <c r="N1" s="5">
+      <c r="O1" s="5">
         <v>2018</v>
       </c>
-      <c r="O1" s="5">
+      <c r="P1" s="5">
         <v>2016</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>40634</v>
       </c>
@@ -1537,14 +1542,15 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="7">
+      <c r="L2" s="5"/>
+      <c r="M2" s="7">
         <v>13</v>
       </c>
-      <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
-    </row>
-    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>40635</v>
       </c>
@@ -1556,18 +1562,19 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="5">
+      <c r="J3" s="5"/>
+      <c r="K3" s="5">
         <v>4</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7">
-        <v>0</v>
-      </c>
-      <c r="M3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
-    </row>
-    <row r="4" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>40636</v>
       </c>
@@ -1579,20 +1586,21 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="5">
+      <c r="J4" s="5"/>
+      <c r="K4" s="5">
         <v>1</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7">
-        <v>0</v>
-      </c>
+      <c r="L4" s="7"/>
       <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
         <v>65</v>
       </c>
-      <c r="N4" s="7"/>
       <c r="O4" s="7"/>
-    </row>
-    <row r="5" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>40637</v>
       </c>
@@ -1604,20 +1612,21 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="5">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5">
         <v>1</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7">
+      <c r="L5" s="7"/>
+      <c r="M5" s="7">
         <v>1</v>
       </c>
-      <c r="M5" s="7">
+      <c r="N5" s="7">
         <v>17</v>
       </c>
-      <c r="N5" s="7"/>
       <c r="O5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>40638</v>
       </c>
@@ -1629,20 +1638,21 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="5">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5">
         <v>1</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7">
+      <c r="L6" s="7"/>
+      <c r="M6" s="7">
         <v>1</v>
       </c>
-      <c r="M6" s="7">
+      <c r="N6" s="7">
         <v>16</v>
       </c>
-      <c r="N6" s="7"/>
       <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>40639</v>
       </c>
@@ -1656,18 +1666,19 @@
       <c r="I7" s="7">
         <v>2</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="7"/>
+      <c r="K7" s="7">
         <v>2</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7">
+      <c r="L7" s="7"/>
+      <c r="M7" s="7">
         <v>2</v>
       </c>
-      <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>40640</v>
       </c>
@@ -1681,20 +1692,20 @@
       <c r="I8" s="7">
         <v>2</v>
       </c>
-      <c r="J8" s="7">
+      <c r="K8" s="7">
         <v>2</v>
       </c>
-      <c r="K8" s="7">
-        <v>0</v>
-      </c>
       <c r="L8" s="7">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
         <v>8</v>
       </c>
-      <c r="M8" s="7">
+      <c r="N8" s="7">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>40641</v>
       </c>
@@ -1710,17 +1721,17 @@
       <c r="I9" s="7">
         <v>2</v>
       </c>
-      <c r="J9" s="7">
-        <v>0</v>
-      </c>
       <c r="K9" s="7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L9" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M9" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>40642</v>
       </c>
@@ -1736,20 +1747,20 @@
       <c r="I10" s="7">
         <v>3</v>
       </c>
-      <c r="J10" s="7">
-        <v>0</v>
-      </c>
       <c r="K10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10" s="7">
         <v>9</v>
       </c>
-      <c r="L10" s="7">
+      <c r="M10" s="7">
         <v>5</v>
       </c>
-      <c r="M10" s="7">
+      <c r="N10" s="7">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>40643</v>
       </c>
@@ -1765,17 +1776,17 @@
       <c r="I11" s="7">
         <v>3</v>
       </c>
-      <c r="J11" s="7">
+      <c r="K11" s="7">
         <v>1</v>
       </c>
-      <c r="K11" s="7">
+      <c r="L11" s="7">
         <v>9</v>
       </c>
-      <c r="L11" s="7">
+      <c r="M11" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>40644</v>
       </c>
@@ -1791,20 +1802,20 @@
       <c r="I12" s="7">
         <v>10</v>
       </c>
-      <c r="J12" s="7">
-        <v>0</v>
-      </c>
       <c r="K12" s="7">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7">
         <v>10</v>
       </c>
-      <c r="L12" s="7">
+      <c r="M12" s="7">
         <v>2</v>
       </c>
-      <c r="M12" s="7">
+      <c r="N12" s="7">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>40645</v>
       </c>
@@ -1821,19 +1832,22 @@
         <v>13</v>
       </c>
       <c r="J13" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K13" s="7">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
         <v>10</v>
       </c>
-      <c r="L13" s="7">
+      <c r="M13" s="7">
         <v>3</v>
       </c>
-      <c r="O13" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>40646</v>
       </c>
@@ -1850,19 +1864,22 @@
         <v>23</v>
       </c>
       <c r="J14" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" s="7">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7">
         <v>11</v>
       </c>
-      <c r="L14" s="7">
+      <c r="M14" s="7">
         <v>3</v>
       </c>
-      <c r="O14" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>40647</v>
       </c>
@@ -1879,22 +1896,25 @@
         <v>24</v>
       </c>
       <c r="J15" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K15" s="7">
+        <v>0</v>
+      </c>
+      <c r="L15" s="7">
         <v>2</v>
       </c>
-      <c r="L15" s="7">
+      <c r="M15" s="7">
         <v>27</v>
       </c>
-      <c r="M15" s="7">
+      <c r="N15" s="7">
         <v>44</v>
       </c>
-      <c r="O15" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>40648</v>
       </c>
@@ -1911,19 +1931,22 @@
         <v>55</v>
       </c>
       <c r="J16" s="7">
+        <v>2</v>
+      </c>
+      <c r="K16" s="7">
         <v>4</v>
       </c>
-      <c r="K16" s="7">
+      <c r="L16" s="7">
         <v>2</v>
       </c>
-      <c r="L16" s="7">
+      <c r="M16" s="7">
         <v>27</v>
       </c>
-      <c r="O16" s="7">
+      <c r="P16" s="7">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>40649</v>
       </c>
@@ -1944,25 +1967,28 @@
         <v>76</v>
       </c>
       <c r="J17" s="7">
+        <v>2</v>
+      </c>
+      <c r="K17" s="7">
         <v>4</v>
       </c>
-      <c r="K17" s="7">
+      <c r="L17" s="7">
         <v>2</v>
       </c>
-      <c r="L17" s="7">
+      <c r="M17" s="7">
         <v>87</v>
       </c>
-      <c r="M17" s="7">
+      <c r="N17" s="7">
         <v>37</v>
       </c>
-      <c r="N17" s="7">
+      <c r="O17" s="7">
         <v>11</v>
       </c>
-      <c r="O17" s="7">
+      <c r="P17" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>40650</v>
       </c>
@@ -1985,22 +2011,25 @@
         <v>76</v>
       </c>
       <c r="J18" s="7">
+        <v>2</v>
+      </c>
+      <c r="K18" s="7">
         <v>15</v>
       </c>
-      <c r="K18" s="7">
+      <c r="L18" s="7">
         <v>13</v>
       </c>
-      <c r="L18" s="7">
+      <c r="M18" s="7">
         <v>87</v>
-      </c>
-      <c r="N18" s="7">
-        <v>3</v>
       </c>
       <c r="O18" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>40651</v>
       </c>
@@ -2025,22 +2054,25 @@
         <v>48</v>
       </c>
       <c r="J19" s="7">
+        <v>10</v>
+      </c>
+      <c r="K19" s="7">
         <v>38</v>
       </c>
-      <c r="K19" s="7">
+      <c r="L19" s="7">
         <v>14</v>
       </c>
-      <c r="L19" s="7">
+      <c r="M19" s="7">
         <v>68</v>
       </c>
-      <c r="N19" s="7">
+      <c r="O19" s="7">
         <v>2</v>
       </c>
-      <c r="O19" s="7">
+      <c r="P19" s="7">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>40652</v>
       </c>
@@ -2065,22 +2097,25 @@
         <v>35</v>
       </c>
       <c r="J20" s="7">
+        <v>11</v>
+      </c>
+      <c r="K20" s="7">
         <v>62</v>
       </c>
-      <c r="K20" s="7">
+      <c r="L20" s="7">
         <v>152</v>
       </c>
-      <c r="L20" s="7">
+      <c r="M20" s="7">
         <v>69</v>
       </c>
-      <c r="N20" s="7">
+      <c r="O20" s="7">
         <v>5</v>
       </c>
-      <c r="O20" s="7">
+      <c r="P20" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>40653</v>
       </c>
@@ -2105,22 +2140,25 @@
         <v>73</v>
       </c>
       <c r="J21" s="7">
+        <v>20</v>
+      </c>
+      <c r="K21" s="7">
         <v>1800</v>
       </c>
-      <c r="K21" s="7">
+      <c r="L21" s="7">
         <v>153</v>
       </c>
-      <c r="L21" s="7">
+      <c r="M21" s="7">
         <v>69</v>
       </c>
-      <c r="N21" s="7">
+      <c r="O21" s="7">
         <v>5</v>
       </c>
-      <c r="O21" s="7">
+      <c r="P21" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>40654</v>
       </c>
@@ -2145,25 +2183,28 @@
         <v>74</v>
       </c>
       <c r="J22" s="7">
+        <v>24</v>
+      </c>
+      <c r="K22" s="7">
         <v>2062</v>
       </c>
-      <c r="K22" s="7">
+      <c r="L22" s="7">
         <v>127</v>
       </c>
-      <c r="L22" s="7">
+      <c r="M22" s="7">
         <v>483</v>
       </c>
-      <c r="M22" s="7">
+      <c r="N22" s="7">
         <v>1541</v>
       </c>
-      <c r="N22" s="7">
+      <c r="O22" s="7">
         <v>6</v>
       </c>
-      <c r="O22" s="7">
+      <c r="P22" s="7">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>40655</v>
       </c>
@@ -2188,22 +2229,25 @@
         <v>234</v>
       </c>
       <c r="J23" s="7">
+        <v>100</v>
+      </c>
+      <c r="K23" s="7">
         <v>4486</v>
       </c>
-      <c r="K23" s="7">
+      <c r="L23" s="7">
         <v>245</v>
       </c>
-      <c r="L23" s="7">
+      <c r="M23" s="7">
         <v>748</v>
       </c>
-      <c r="N23" s="7">
+      <c r="O23" s="7">
         <v>7</v>
       </c>
-      <c r="O23" s="7">
+      <c r="P23" s="7">
         <v>32.799999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>40656</v>
       </c>
@@ -2230,25 +2274,28 @@
         <v>564</v>
       </c>
       <c r="J24" s="7">
+        <v>112</v>
+      </c>
+      <c r="K24" s="7">
         <v>6352</v>
       </c>
-      <c r="K24" s="7">
+      <c r="L24" s="7">
         <v>200</v>
       </c>
-      <c r="L24" s="7">
+      <c r="M24" s="7">
         <v>380</v>
       </c>
-      <c r="M24" s="7">
+      <c r="N24" s="7">
         <v>2041</v>
       </c>
-      <c r="N24" s="7">
+      <c r="O24" s="7">
         <v>8</v>
       </c>
-      <c r="O24" s="7">
+      <c r="P24" s="7">
         <v>28.6</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>40657</v>
       </c>
@@ -2273,25 +2320,28 @@
         <v>458</v>
       </c>
       <c r="J25" s="7">
+        <v>158</v>
+      </c>
+      <c r="K25" s="7">
         <v>8818</v>
       </c>
-      <c r="K25" s="7">
+      <c r="L25" s="7">
         <v>61</v>
       </c>
-      <c r="L25" s="7">
+      <c r="M25" s="7">
         <v>381</v>
       </c>
-      <c r="M25" s="7">
+      <c r="N25" s="7">
         <v>3600</v>
       </c>
-      <c r="N25" s="7">
+      <c r="O25" s="7">
         <v>10</v>
       </c>
-      <c r="O25" s="7">
+      <c r="P25" s="7">
         <v>24.4</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>40658</v>
       </c>
@@ -2318,25 +2368,28 @@
         <v>363</v>
       </c>
       <c r="J26" s="7">
+        <v>321</v>
+      </c>
+      <c r="K26" s="7">
         <v>17758</v>
       </c>
-      <c r="K26" s="7">
+      <c r="L26" s="7">
         <v>460</v>
       </c>
-      <c r="L26" s="7">
+      <c r="M26" s="7">
         <v>392</v>
       </c>
-      <c r="M26" s="7">
+      <c r="N26" s="7">
         <v>1210</v>
       </c>
-      <c r="N26" s="7">
+      <c r="O26" s="7">
         <v>12</v>
       </c>
-      <c r="O26" s="7">
+      <c r="P26" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>40659</v>
       </c>
@@ -2363,25 +2416,28 @@
         <v>669</v>
       </c>
       <c r="J27" s="7">
+        <v>300</v>
+      </c>
+      <c r="K27" s="7">
         <v>13011</v>
       </c>
-      <c r="K27" s="7">
+      <c r="L27" s="7">
         <v>795</v>
       </c>
-      <c r="L27" s="7">
+      <c r="M27" s="7">
         <v>449</v>
       </c>
-      <c r="M27" s="7">
+      <c r="N27" s="7">
         <v>649</v>
       </c>
-      <c r="N27" s="7">
+      <c r="O27" s="7">
         <v>15</v>
       </c>
-      <c r="O27" s="7">
+      <c r="P27" s="7">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>40660</v>
       </c>
@@ -2408,25 +2464,28 @@
         <v>1809</v>
       </c>
       <c r="J28" s="7">
+        <v>492</v>
+      </c>
+      <c r="K28" s="7">
         <v>15671</v>
       </c>
-      <c r="K28" s="7">
+      <c r="L28" s="7">
         <v>480</v>
       </c>
-      <c r="L28" s="7">
+      <c r="M28" s="7">
         <v>450</v>
       </c>
-      <c r="M28" s="7">
+      <c r="N28" s="7">
         <v>3337</v>
       </c>
-      <c r="N28" s="7">
+      <c r="O28" s="7">
         <v>16</v>
       </c>
-      <c r="O28" s="7">
+      <c r="P28" s="7">
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>40661</v>
       </c>
@@ -2453,25 +2512,28 @@
         <v>2276</v>
       </c>
       <c r="J29" s="7">
+        <v>230</v>
+      </c>
+      <c r="K29" s="7">
         <v>18407</v>
       </c>
-      <c r="K29" s="7">
+      <c r="L29" s="7">
         <v>875</v>
       </c>
-      <c r="L29" s="7">
+      <c r="M29" s="7">
         <v>911</v>
       </c>
-      <c r="M29" s="7">
+      <c r="N29" s="7">
         <v>1929</v>
       </c>
-      <c r="N29" s="7">
+      <c r="O29" s="7">
         <v>800</v>
       </c>
-      <c r="O29" s="7">
+      <c r="P29" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>40662</v>
       </c>
@@ -2500,25 +2562,28 @@
         <v>2100</v>
       </c>
       <c r="J30" s="7">
+        <v>194</v>
+      </c>
+      <c r="K30" s="7">
         <v>11338</v>
       </c>
-      <c r="K30" s="7">
+      <c r="L30" s="7">
         <v>715</v>
       </c>
-      <c r="L30" s="7">
+      <c r="M30" s="7">
         <v>171</v>
       </c>
-      <c r="M30" s="7">
+      <c r="N30" s="7">
         <v>1005</v>
       </c>
-      <c r="N30" s="7">
+      <c r="O30" s="7">
         <v>1408</v>
       </c>
-      <c r="O30" s="7">
+      <c r="P30" s="7">
         <v>229.34</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>40663</v>
       </c>
@@ -2547,25 +2612,28 @@
         <v>3114</v>
       </c>
       <c r="J31" s="7">
+        <v>115</v>
+      </c>
+      <c r="K31" s="7">
         <v>8358</v>
       </c>
-      <c r="K31" s="7">
+      <c r="L31" s="7">
         <v>1054</v>
       </c>
-      <c r="L31" s="7">
+      <c r="M31" s="7">
         <v>324</v>
       </c>
-      <c r="M31" s="7">
+      <c r="N31" s="7">
         <v>1715</v>
       </c>
-      <c r="N31" s="7">
+      <c r="O31" s="7">
         <v>2941</v>
       </c>
-      <c r="O31" s="7">
+      <c r="P31" s="7">
         <v>396</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>40664</v>
       </c>
@@ -2594,25 +2662,28 @@
         <v>973</v>
       </c>
       <c r="J32" s="7">
+        <v>34</v>
+      </c>
+      <c r="K32" s="7">
         <v>14238</v>
       </c>
-      <c r="K32" s="7">
+      <c r="L32" s="7">
         <v>877</v>
       </c>
-      <c r="L32" s="7">
+      <c r="M32" s="7">
         <v>171</v>
       </c>
-      <c r="M32" s="7">
+      <c r="N32" s="7">
         <v>1410</v>
       </c>
-      <c r="N32" s="7">
+      <c r="O32" s="7">
         <v>1166</v>
       </c>
-      <c r="O32" s="7">
+      <c r="P32" s="7">
         <v>384</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>40665</v>
       </c>
@@ -2639,25 +2710,28 @@
         <v>2303</v>
       </c>
       <c r="J33" s="7">
+        <v>38</v>
+      </c>
+      <c r="K33" s="7">
         <v>9068</v>
       </c>
-      <c r="K33" s="7">
+      <c r="L33" s="7">
         <v>1009</v>
       </c>
-      <c r="L33" s="7">
+      <c r="M33" s="7">
         <v>217</v>
       </c>
-      <c r="M33" s="7">
+      <c r="N33" s="7">
         <v>4032</v>
       </c>
-      <c r="N33" s="7">
+      <c r="O33" s="7">
         <v>3568</v>
       </c>
-      <c r="O33" s="7">
+      <c r="P33" s="7">
         <v>556</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>40666</v>
       </c>
@@ -2686,25 +2760,28 @@
         <v>2305</v>
       </c>
       <c r="J34" s="7">
+        <v>11</v>
+      </c>
+      <c r="K34" s="7">
         <v>9438</v>
       </c>
-      <c r="K34" s="7">
+      <c r="L34" s="7">
         <v>991</v>
       </c>
-      <c r="L34" s="7">
+      <c r="M34" s="7">
         <v>145</v>
       </c>
-      <c r="M34" s="7">
+      <c r="N34" s="7">
         <v>2036</v>
       </c>
-      <c r="N34" s="7">
+      <c r="O34" s="7">
         <v>1536</v>
       </c>
-      <c r="O34" s="7">
+      <c r="P34" s="7">
         <v>512</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>40667</v>
       </c>
@@ -2733,25 +2810,28 @@
         <v>2905</v>
       </c>
       <c r="J35" s="7">
+        <v>214</v>
+      </c>
+      <c r="K35" s="7">
         <v>10067</v>
       </c>
-      <c r="K35" s="7">
+      <c r="L35" s="7">
         <v>706</v>
       </c>
-      <c r="L35" s="7">
+      <c r="M35" s="7">
         <v>151</v>
       </c>
-      <c r="M35" s="7">
+      <c r="N35" s="7">
         <v>1867</v>
       </c>
-      <c r="N35" s="7">
+      <c r="O35" s="7">
         <v>6278</v>
       </c>
-      <c r="O35" s="7">
+      <c r="P35" s="7">
         <v>918</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>40668</v>
       </c>
@@ -2780,25 +2860,28 @@
         <v>6890</v>
       </c>
       <c r="J36" s="7">
+        <v>65</v>
+      </c>
+      <c r="K36" s="7">
         <v>11378</v>
       </c>
-      <c r="K36" s="7">
+      <c r="L36" s="7">
         <v>895</v>
       </c>
-      <c r="L36" s="7">
+      <c r="M36" s="7">
         <v>172</v>
       </c>
-      <c r="M36" s="7">
+      <c r="N36" s="7">
         <v>1039</v>
       </c>
-      <c r="N36" s="7">
+      <c r="O36" s="7">
         <v>4500</v>
       </c>
-      <c r="O36" s="7">
+      <c r="P36" s="7">
         <v>976</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>40669</v>
       </c>
@@ -2825,25 +2908,28 @@
         <v>4646</v>
       </c>
       <c r="J37" s="7">
+        <v>67</v>
+      </c>
+      <c r="K37" s="7">
         <v>8610</v>
       </c>
-      <c r="K37" s="7">
+      <c r="L37" s="7">
         <v>466</v>
       </c>
-      <c r="L37" s="7">
+      <c r="M37" s="7">
         <v>173</v>
       </c>
-      <c r="M37" s="7">
+      <c r="N37" s="7">
         <v>5070</v>
       </c>
-      <c r="N37" s="7">
+      <c r="O37" s="7">
         <v>5430</v>
       </c>
-      <c r="O37" s="7">
+      <c r="P37" s="7">
         <v>1647</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>40670</v>
       </c>
@@ -2872,25 +2958,28 @@
         <v>7265</v>
       </c>
       <c r="J38" s="7">
+        <v>125</v>
+      </c>
+      <c r="K38" s="7">
         <v>14399</v>
       </c>
-      <c r="K38" s="7">
+      <c r="L38" s="7">
         <v>590</v>
       </c>
-      <c r="L38" s="7">
+      <c r="M38" s="7">
         <v>175</v>
       </c>
-      <c r="M38" s="7">
+      <c r="N38" s="7">
         <v>1467</v>
       </c>
-      <c r="N38" s="7">
+      <c r="O38" s="7">
         <v>9311</v>
       </c>
-      <c r="O38" s="7">
+      <c r="P38" s="7">
         <v>1256</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>40671</v>
       </c>
@@ -2919,25 +3008,28 @@
         <v>4801</v>
       </c>
       <c r="J39" s="7">
+        <v>80</v>
+      </c>
+      <c r="K39" s="7">
         <v>26529</v>
       </c>
-      <c r="K39" s="7">
+      <c r="L39" s="7">
         <v>1345</v>
       </c>
-      <c r="L39" s="7">
+      <c r="M39" s="7">
         <v>94</v>
       </c>
-      <c r="M39" s="7">
+      <c r="N39" s="7">
         <v>2092</v>
       </c>
-      <c r="N39" s="7">
+      <c r="O39" s="7">
         <v>6797</v>
       </c>
-      <c r="O39" s="7">
+      <c r="P39" s="7">
         <v>504</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>40672</v>
       </c>
@@ -2966,25 +3058,28 @@
         <v>3658</v>
       </c>
       <c r="J40" s="7">
+        <v>34</v>
+      </c>
+      <c r="K40" s="7">
         <v>17025</v>
       </c>
-      <c r="K40" s="7">
+      <c r="L40" s="7">
         <v>861</v>
       </c>
-      <c r="L40" s="7">
+      <c r="M40" s="7">
         <v>250</v>
       </c>
-      <c r="M40" s="7">
+      <c r="N40" s="7">
         <v>1896</v>
       </c>
-      <c r="N40" s="7">
+      <c r="O40" s="7">
         <v>5887</v>
       </c>
-      <c r="O40" s="7">
+      <c r="P40" s="7">
         <v>724</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>40673</v>
       </c>
@@ -3013,25 +3108,28 @@
         <v>2293</v>
       </c>
       <c r="J41" s="7">
+        <v>34</v>
+      </c>
+      <c r="K41" s="7">
         <v>15238</v>
       </c>
-      <c r="K41" s="7">
+      <c r="L41" s="7">
         <v>1061</v>
       </c>
-      <c r="L41" s="7">
+      <c r="M41" s="7">
         <v>265</v>
       </c>
-      <c r="M41" s="7">
+      <c r="N41" s="7">
         <v>1599</v>
       </c>
-      <c r="N41" s="7">
+      <c r="O41" s="7">
         <v>3027</v>
       </c>
-      <c r="O41" s="7">
+      <c r="P41" s="7">
         <v>1464</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>40674</v>
       </c>
@@ -3058,25 +3156,28 @@
         <v>1920</v>
       </c>
       <c r="J42" s="7">
+        <v>39</v>
+      </c>
+      <c r="K42" s="7">
         <v>6919</v>
       </c>
-      <c r="K42" s="7">
+      <c r="L42" s="7">
         <v>1200</v>
       </c>
-      <c r="L42" s="7">
+      <c r="M42" s="7">
         <v>303</v>
       </c>
-      <c r="M42" s="7">
+      <c r="N42" s="7">
         <v>2508</v>
       </c>
-      <c r="N42" s="7">
+      <c r="O42" s="7">
         <v>2930</v>
       </c>
-      <c r="O42" s="7">
+      <c r="P42" s="7">
         <v>1418</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>40675</v>
       </c>
@@ -3103,25 +3204,28 @@
         <v>1681</v>
       </c>
       <c r="J43" s="7">
+        <v>145</v>
+      </c>
+      <c r="K43" s="7">
         <v>2850</v>
       </c>
-      <c r="K43" s="7">
+      <c r="L43" s="7">
         <v>2470</v>
       </c>
-      <c r="L43" s="7">
+      <c r="M43" s="7">
         <v>658</v>
       </c>
-      <c r="M43" s="7">
+      <c r="N43" s="7">
         <v>1715</v>
       </c>
-      <c r="N43" s="7">
+      <c r="O43" s="7">
         <v>4979</v>
       </c>
-      <c r="O43" s="7">
+      <c r="P43" s="7">
         <v>1388</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>40676</v>
       </c>
@@ -3150,25 +3254,28 @@
         <v>3000</v>
       </c>
       <c r="J44" s="7">
+        <v>83</v>
+      </c>
+      <c r="K44" s="7">
         <v>3421</v>
       </c>
-      <c r="K44" s="7">
+      <c r="L44" s="7">
         <v>1595</v>
       </c>
-      <c r="L44" s="7">
+      <c r="M44" s="7">
         <v>266</v>
       </c>
-      <c r="M44" s="7">
+      <c r="N44" s="7">
         <v>1718</v>
       </c>
-      <c r="N44" s="7">
+      <c r="O44" s="7">
         <v>3816</v>
       </c>
-      <c r="O44" s="7">
+      <c r="P44" s="7">
         <v>719</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>40677</v>
       </c>
@@ -3195,25 +3302,28 @@
         <v>5436</v>
       </c>
       <c r="J45" s="7">
+        <v>85</v>
+      </c>
+      <c r="K45" s="7">
         <v>2867</v>
       </c>
-      <c r="K45" s="7">
+      <c r="L45" s="7">
         <v>2517</v>
       </c>
-      <c r="L45" s="7">
+      <c r="M45" s="7">
         <v>317</v>
       </c>
-      <c r="M45" s="7">
+      <c r="N45" s="7">
         <v>806</v>
       </c>
-      <c r="N45" s="7">
+      <c r="O45" s="7">
         <v>2274</v>
       </c>
-      <c r="O45" s="7">
+      <c r="P45" s="7">
         <v>580</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>40678</v>
       </c>
@@ -3240,25 +3350,28 @@
         <v>5207</v>
       </c>
       <c r="J46" s="7">
+        <v>107</v>
+      </c>
+      <c r="K46" s="7">
         <v>3050</v>
       </c>
-      <c r="K46" s="7">
+      <c r="L46" s="7">
         <v>1270</v>
       </c>
-      <c r="L46" s="7">
+      <c r="M46" s="7">
         <v>36</v>
       </c>
-      <c r="M46" s="7">
+      <c r="N46" s="7">
         <v>750</v>
       </c>
-      <c r="N46" s="7">
+      <c r="O46" s="7">
         <v>2833</v>
       </c>
-      <c r="O46" s="7">
+      <c r="P46" s="7">
         <v>544</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>40679</v>
       </c>
@@ -3285,25 +3398,28 @@
         <v>4475</v>
       </c>
       <c r="J47" s="7">
+        <v>190</v>
+      </c>
+      <c r="K47" s="7">
         <v>2903</v>
       </c>
-      <c r="K47" s="7">
+      <c r="L47" s="7">
         <v>1889</v>
       </c>
-      <c r="L47" s="7">
+      <c r="M47" s="7">
         <v>105</v>
       </c>
-      <c r="M47" s="7">
+      <c r="N47" s="7">
         <v>1198</v>
       </c>
-      <c r="N47" s="7">
+      <c r="O47" s="7">
         <v>1381</v>
       </c>
-      <c r="O47" s="7">
+      <c r="P47" s="7">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>40680</v>
       </c>
@@ -3330,25 +3446,28 @@
         <v>3011</v>
       </c>
       <c r="J48" s="7">
+        <v>204</v>
+      </c>
+      <c r="K48" s="7">
         <v>3837</v>
       </c>
-      <c r="K48" s="7">
+      <c r="L48" s="7">
         <v>1483</v>
       </c>
-      <c r="L48" s="7">
+      <c r="M48" s="7">
         <v>105</v>
       </c>
-      <c r="M48" s="7">
+      <c r="N48" s="7">
         <v>85</v>
       </c>
-      <c r="N48" s="7">
+      <c r="O48" s="7">
         <v>1184</v>
       </c>
-      <c r="O48" s="7">
+      <c r="P48" s="7">
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>40681</v>
       </c>
@@ -3375,25 +3494,28 @@
         <v>1540</v>
       </c>
       <c r="J49" s="7">
+        <v>481</v>
+      </c>
+      <c r="K49" s="7">
         <v>2094</v>
       </c>
-      <c r="K49" s="7">
+      <c r="L49" s="7">
         <v>892</v>
       </c>
-      <c r="L49" s="7">
+      <c r="M49" s="7">
         <v>200</v>
       </c>
-      <c r="M49" s="7">
+      <c r="N49" s="7">
         <v>2257</v>
       </c>
-      <c r="N49" s="7">
+      <c r="O49" s="7">
         <v>672</v>
       </c>
-      <c r="O49" s="7">
+      <c r="P49" s="7">
         <v>250</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>40682</v>
       </c>
@@ -3420,25 +3542,28 @@
         <v>984</v>
       </c>
       <c r="J50" s="7">
+        <v>1797</v>
+      </c>
+      <c r="K50" s="7">
         <v>3923</v>
       </c>
-      <c r="K50" s="7">
+      <c r="L50" s="7">
         <v>1043</v>
       </c>
-      <c r="L50" s="7">
+      <c r="M50" s="7">
         <v>200</v>
       </c>
-      <c r="M50" s="7">
+      <c r="N50" s="7">
         <v>1236</v>
       </c>
-      <c r="N50" s="7">
+      <c r="O50" s="7">
         <v>346</v>
       </c>
-      <c r="O50" s="7">
+      <c r="P50" s="7">
         <v>436</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>40683</v>
       </c>
@@ -3465,25 +3590,28 @@
         <v>1009</v>
       </c>
       <c r="J51" s="7">
+        <v>959</v>
+      </c>
+      <c r="K51" s="7">
         <v>2025</v>
       </c>
-      <c r="K51" s="7">
+      <c r="L51" s="7">
         <v>1207</v>
       </c>
-      <c r="L51" s="7">
+      <c r="M51" s="7">
         <v>141</v>
       </c>
-      <c r="M51" s="7">
+      <c r="N51" s="7">
         <v>428</v>
       </c>
-      <c r="N51" s="7">
+      <c r="O51" s="7">
         <v>452</v>
       </c>
-      <c r="O51" s="7">
+      <c r="P51" s="7">
         <v>460</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>40684</v>
       </c>
@@ -3508,22 +3636,25 @@
         <v>421</v>
       </c>
       <c r="J52" s="7">
+        <v>986</v>
+      </c>
+      <c r="K52" s="7">
         <v>2009</v>
       </c>
-      <c r="K52" s="7">
+      <c r="L52" s="7">
         <v>750</v>
       </c>
-      <c r="L52" s="7">
+      <c r="M52" s="7">
         <v>58</v>
       </c>
-      <c r="N52" s="7">
+      <c r="O52" s="7">
         <v>500</v>
       </c>
-      <c r="O52" s="7">
+      <c r="P52" s="7">
         <v>380</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>40685</v>
       </c>
@@ -3546,25 +3677,28 @@
         <v>1504</v>
       </c>
       <c r="J53" s="7">
+        <v>508</v>
+      </c>
+      <c r="K53" s="7">
         <v>3401</v>
       </c>
-      <c r="K53" s="7">
+      <c r="L53" s="7">
         <v>2356</v>
       </c>
-      <c r="L53" s="7">
+      <c r="M53" s="7">
         <v>59</v>
       </c>
-      <c r="M53" s="7">
+      <c r="N53" s="7">
         <v>552</v>
       </c>
-      <c r="N53" s="7">
+      <c r="O53" s="7">
         <v>551</v>
       </c>
-      <c r="O53" s="7">
+      <c r="P53" s="7">
         <v>352</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>40686</v>
       </c>
@@ -3587,25 +3721,28 @@
         <v>1685</v>
       </c>
       <c r="J54" s="7">
+        <v>653</v>
+      </c>
+      <c r="K54" s="7">
         <v>2374</v>
       </c>
-      <c r="K54" s="7">
+      <c r="L54" s="7">
         <v>1390</v>
       </c>
-      <c r="L54" s="7">
+      <c r="M54" s="7">
         <v>9</v>
       </c>
-      <c r="M54" s="7">
+      <c r="N54" s="7">
         <v>704</v>
       </c>
-      <c r="N54" s="7">
+      <c r="O54" s="7">
         <v>311</v>
       </c>
-      <c r="O54" s="7">
+      <c r="P54" s="7">
         <v>324</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>40687</v>
       </c>
@@ -3626,22 +3763,25 @@
         <v>2358</v>
       </c>
       <c r="J55" s="7">
+        <v>450</v>
+      </c>
+      <c r="K55" s="7">
         <v>2374</v>
       </c>
-      <c r="K55" s="7">
+      <c r="L55" s="7">
         <v>1089</v>
       </c>
-      <c r="L55" s="7">
+      <c r="M55" s="7">
         <v>21</v>
       </c>
-      <c r="N55" s="7">
+      <c r="O55" s="7">
         <v>350</v>
       </c>
-      <c r="O55" s="7">
+      <c r="P55" s="7">
         <v>395</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>40688</v>
       </c>
@@ -3662,22 +3802,25 @@
         <v>1855</v>
       </c>
       <c r="J56" s="7">
+        <v>1135</v>
+      </c>
+      <c r="K56" s="7">
         <v>900</v>
       </c>
-      <c r="K56" s="7">
+      <c r="L56" s="7">
         <v>561</v>
       </c>
-      <c r="L56" s="7">
+      <c r="M56" s="7">
         <v>21</v>
       </c>
-      <c r="N56" s="7">
+      <c r="O56" s="7">
         <v>350</v>
       </c>
-      <c r="O56" s="7">
+      <c r="P56" s="7">
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>40689</v>
       </c>
@@ -3698,25 +3841,28 @@
         <v>1302</v>
       </c>
       <c r="J57" s="7">
+        <v>1154</v>
+      </c>
+      <c r="K57" s="7">
         <v>700</v>
       </c>
-      <c r="K57" s="7">
+      <c r="L57" s="7">
         <v>206</v>
       </c>
-      <c r="L57" s="7">
+      <c r="M57" s="7">
         <v>21</v>
       </c>
-      <c r="M57" s="7">
+      <c r="N57" s="7">
         <v>681</v>
       </c>
-      <c r="N57" s="7">
+      <c r="O57" s="7">
         <v>307</v>
       </c>
-      <c r="O57" s="7">
+      <c r="P57" s="7">
         <v>240</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>40690</v>
       </c>
@@ -3737,25 +3883,28 @@
         <v>1373</v>
       </c>
       <c r="J58" s="7">
+        <v>654</v>
+      </c>
+      <c r="K58" s="7">
         <v>450</v>
       </c>
-      <c r="K58" s="7">
+      <c r="L58" s="7">
         <v>134</v>
       </c>
-      <c r="L58" s="7">
+      <c r="M58" s="7">
         <v>21</v>
       </c>
-      <c r="M58" s="7">
+      <c r="N58" s="7">
         <v>173</v>
       </c>
-      <c r="N58" s="7">
+      <c r="O58" s="7">
         <v>160</v>
       </c>
-      <c r="O58" s="7">
+      <c r="P58" s="7">
         <v>266</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>40691</v>
       </c>
@@ -3776,25 +3925,28 @@
         <v>1989</v>
       </c>
       <c r="J59" s="7">
+        <v>401</v>
+      </c>
+      <c r="K59" s="7">
         <v>348</v>
       </c>
-      <c r="K59" s="7">
+      <c r="L59" s="7">
         <v>133</v>
       </c>
-      <c r="L59" s="7">
+      <c r="M59" s="7">
         <v>21</v>
       </c>
-      <c r="M59" s="7">
+      <c r="N59" s="7">
         <v>188</v>
       </c>
-      <c r="N59" s="7">
+      <c r="O59" s="7">
         <v>57</v>
       </c>
-      <c r="O59" s="7">
+      <c r="P59" s="7">
         <v>184</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>40692</v>
       </c>
@@ -3815,22 +3967,25 @@
         <v>2659</v>
       </c>
       <c r="J60" s="7">
+        <v>478</v>
+      </c>
+      <c r="K60" s="7">
         <v>928</v>
       </c>
-      <c r="K60" s="7">
+      <c r="L60" s="7">
         <v>289</v>
       </c>
-      <c r="L60" s="7">
+      <c r="M60" s="7">
         <v>21</v>
       </c>
-      <c r="N60" s="7">
+      <c r="O60" s="7">
         <v>57</v>
       </c>
-      <c r="O60" s="7">
+      <c r="P60" s="7">
         <v>156</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>40693</v>
       </c>
@@ -3851,22 +4006,25 @@
         <v>2216</v>
       </c>
       <c r="J61" s="7">
+        <v>852</v>
+      </c>
+      <c r="K61" s="7">
         <v>508</v>
       </c>
-      <c r="K61" s="7">
+      <c r="L61" s="7">
         <v>333</v>
       </c>
-      <c r="L61" s="7">
+      <c r="M61" s="7">
         <v>6</v>
       </c>
-      <c r="N61" s="7">
+      <c r="O61" s="7">
         <v>57</v>
       </c>
-      <c r="O61" s="7">
+      <c r="P61" s="7">
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>40694</v>
       </c>
@@ -3887,25 +4045,28 @@
         <v>23</v>
       </c>
       <c r="J62" s="7">
+        <v>687</v>
+      </c>
+      <c r="K62" s="7">
         <v>200</v>
       </c>
-      <c r="K62" s="7">
+      <c r="L62" s="7">
         <v>136</v>
       </c>
-      <c r="L62" s="7">
+      <c r="M62" s="7">
         <v>7</v>
       </c>
-      <c r="M62" s="7">
+      <c r="N62" s="7">
         <v>153</v>
       </c>
-      <c r="N62" s="7">
+      <c r="O62" s="7">
         <v>95</v>
       </c>
-      <c r="O62" s="7">
+      <c r="P62" s="7">
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>40695</v>
       </c>
@@ -3924,22 +4085,25 @@
         <v>22</v>
       </c>
       <c r="J63" s="7">
+        <v>668</v>
+      </c>
+      <c r="K63" s="7">
         <v>187</v>
       </c>
-      <c r="K63" s="7">
+      <c r="L63" s="7">
         <v>135</v>
       </c>
-      <c r="L63" s="7">
+      <c r="M63" s="7">
         <v>7</v>
       </c>
-      <c r="N63" s="7">
+      <c r="O63" s="7">
         <v>124</v>
       </c>
-      <c r="O63" s="7">
+      <c r="P63" s="7">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>40696</v>
       </c>
@@ -3958,25 +4122,28 @@
         <v>22</v>
       </c>
       <c r="J64" s="7">
+        <v>1028</v>
+      </c>
+      <c r="K64" s="7">
         <v>190</v>
       </c>
-      <c r="K64" s="7">
+      <c r="L64" s="7">
         <v>80</v>
       </c>
-      <c r="L64" s="7">
+      <c r="M64" s="7">
         <v>7</v>
       </c>
-      <c r="M64" s="7">
+      <c r="N64" s="7">
         <v>31</v>
       </c>
-      <c r="N64" s="7">
+      <c r="O64" s="7">
         <v>166</v>
       </c>
-      <c r="O64" s="7">
+      <c r="P64" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>40697</v>
       </c>
@@ -3995,22 +4162,25 @@
         <v>24</v>
       </c>
       <c r="J65" s="7">
+        <v>1308</v>
+      </c>
+      <c r="K65" s="7">
         <v>165</v>
       </c>
-      <c r="K65" s="7">
+      <c r="L65" s="7">
         <v>159</v>
       </c>
-      <c r="L65" s="7">
+      <c r="M65" s="7">
         <v>45</v>
       </c>
-      <c r="N65" s="7">
+      <c r="O65" s="7">
         <v>121</v>
       </c>
-      <c r="O65" s="7">
+      <c r="P65" s="7">
         <v>67.36</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>40698</v>
       </c>
@@ -4029,22 +4199,25 @@
         <v>116</v>
       </c>
       <c r="J66" s="7">
+        <v>186</v>
+      </c>
+      <c r="K66" s="7">
         <v>150</v>
       </c>
-      <c r="K66" s="7">
+      <c r="L66" s="7">
         <v>25</v>
       </c>
-      <c r="L66" s="7">
+      <c r="M66" s="7">
         <v>4</v>
       </c>
-      <c r="N66" s="7">
+      <c r="O66" s="7">
         <v>25</v>
       </c>
-      <c r="O66" s="7">
+      <c r="P66" s="7">
         <v>75.44</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>40699</v>
       </c>
@@ -4063,22 +4236,25 @@
         <v>13</v>
       </c>
       <c r="J67" s="7">
+        <v>166</v>
+      </c>
+      <c r="K67" s="7">
         <v>125</v>
       </c>
-      <c r="L67" s="7">
+      <c r="M67" s="7">
         <v>5</v>
       </c>
-      <c r="M67" s="7">
+      <c r="N67" s="7">
         <v>109</v>
       </c>
-      <c r="N67" s="7">
+      <c r="O67" s="7">
         <v>22</v>
       </c>
-      <c r="O67" s="7">
+      <c r="P67" s="7">
         <v>83.6</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>40700</v>
       </c>
@@ -4093,126 +4269,167 @@
         <v>13</v>
       </c>
       <c r="J68" s="7">
+        <v>211</v>
+      </c>
+      <c r="K68" s="7">
         <v>174</v>
       </c>
-      <c r="L68" s="7">
+      <c r="M68" s="7">
         <v>5</v>
       </c>
-      <c r="N68" s="7">
+      <c r="O68" s="7">
         <v>120</v>
       </c>
-      <c r="O68" s="7">
+      <c r="P68" s="7">
         <v>91.76</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>40701</v>
       </c>
       <c r="I69" s="7">
         <v>12</v>
       </c>
-      <c r="L69" s="7">
+      <c r="J69" s="7">
+        <v>261</v>
+      </c>
+      <c r="M69" s="7">
         <v>5</v>
       </c>
-      <c r="M69" s="7">
+      <c r="N69" s="7">
         <v>198</v>
       </c>
-      <c r="N69" s="7">
+      <c r="O69" s="7">
         <v>62</v>
       </c>
-      <c r="O69" s="7">
+      <c r="P69" s="7">
         <v>99.84</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
         <v>40702</v>
       </c>
       <c r="I70" s="7">
         <v>11</v>
       </c>
-      <c r="L70" s="7">
+      <c r="J70" s="7">
+        <v>89</v>
+      </c>
+      <c r="M70" s="7">
         <v>6</v>
       </c>
-      <c r="N70" s="7">
+      <c r="O70" s="7">
         <v>753</v>
       </c>
-      <c r="O70" s="7">
+      <c r="P70" s="7">
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>40703</v>
       </c>
       <c r="I71" s="7">
         <v>21</v>
       </c>
-      <c r="N71" s="7">
+      <c r="J71" s="7">
+        <v>102</v>
+      </c>
+      <c r="O71" s="7">
         <v>164</v>
       </c>
-      <c r="O71" s="7">
+      <c r="P71" s="7">
         <v>268</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>40704</v>
       </c>
-      <c r="N72" s="7">
+      <c r="J72" s="7">
+        <v>62</v>
+      </c>
+      <c r="O72" s="7">
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>40705</v>
       </c>
-      <c r="N73" s="7">
+      <c r="J73" s="7">
+        <v>140</v>
+      </c>
+      <c r="O73" s="7">
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>40706</v>
       </c>
-      <c r="N74" s="7">
+      <c r="J74" s="7">
+        <v>72</v>
+      </c>
+      <c r="O74" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>40707</v>
       </c>
-      <c r="M75" s="7">
+      <c r="J75" s="7">
+        <v>113</v>
+      </c>
+      <c r="N75" s="7">
         <v>100</v>
       </c>
-      <c r="N75" s="7">
+      <c r="O75" s="7">
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>40708</v>
       </c>
-      <c r="N76" s="7">
+      <c r="J76" s="7">
+        <v>44</v>
+      </c>
+      <c r="O76" s="7">
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>40709</v>
       </c>
-      <c r="N77" s="7">
+      <c r="J77" s="7">
+        <v>63</v>
+      </c>
+      <c r="O77" s="7">
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>40710</v>
       </c>
-      <c r="N78" s="7">
+      <c r="J78" s="7">
+        <v>50</v>
+      </c>
+      <c r="O78" s="7">
         <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" s="6">
+        <v>40711</v>
+      </c>
+      <c r="J79" s="7">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -4222,18 +4439,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E34761F-625A-4051-AABB-744B53998DE3}">
-  <dimension ref="A1:B137"/>
+  <dimension ref="A1:B167"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4241,7 +4458,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>44309</v>
       </c>
@@ -4249,7 +4466,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>44310</v>
       </c>
@@ -4257,7 +4474,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>44311</v>
       </c>
@@ -4265,7 +4482,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>44312</v>
       </c>
@@ -4273,7 +4490,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>44313</v>
       </c>
@@ -4281,7 +4498,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>44314</v>
       </c>
@@ -4289,7 +4506,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>44315</v>
       </c>
@@ -4297,7 +4514,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>44316</v>
       </c>
@@ -4305,7 +4522,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>44317</v>
       </c>
@@ -4313,7 +4530,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>44318</v>
       </c>
@@ -4321,7 +4538,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>44319</v>
       </c>
@@ -4329,7 +4546,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>44320</v>
       </c>
@@ -4337,7 +4554,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>44321</v>
       </c>
@@ -4345,7 +4562,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>44322</v>
       </c>
@@ -4353,7 +4570,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>44323</v>
       </c>
@@ -4361,7 +4578,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>44324</v>
       </c>
@@ -4369,7 +4586,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>44325</v>
       </c>
@@ -4377,7 +4594,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>44326</v>
       </c>
@@ -4385,7 +4602,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>44327</v>
       </c>
@@ -4393,7 +4610,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>44328</v>
       </c>
@@ -4401,12 +4618,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>44329</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>44330</v>
       </c>
@@ -4414,7 +4631,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>44331</v>
       </c>
@@ -4422,7 +4639,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>44332</v>
       </c>
@@ -4430,7 +4647,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>44333</v>
       </c>
@@ -4438,7 +4655,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>44334</v>
       </c>
@@ -4446,7 +4663,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>44335</v>
       </c>
@@ -4454,12 +4671,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>44336</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>44337</v>
       </c>
@@ -4467,7 +4684,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>44338</v>
       </c>
@@ -4475,7 +4692,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>44339</v>
       </c>
@@ -4483,7 +4700,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>44340</v>
       </c>
@@ -4491,7 +4708,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>44341</v>
       </c>
@@ -4499,7 +4716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>44342</v>
       </c>
@@ -4507,12 +4724,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>44343</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>44344</v>
       </c>
@@ -4520,7 +4737,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>44345</v>
       </c>
@@ -4528,7 +4745,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>44346</v>
       </c>
@@ -4536,7 +4753,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>44347</v>
       </c>
@@ -4544,7 +4761,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>44348</v>
       </c>
@@ -4552,7 +4769,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>44349</v>
       </c>
@@ -4560,7 +4777,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>44350</v>
       </c>
@@ -4568,7 +4785,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>44351</v>
       </c>
@@ -4576,7 +4793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44674</v>
       </c>
@@ -4584,7 +4801,7 @@
         <v>2277</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44675</v>
       </c>
@@ -4592,7 +4809,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>44676</v>
       </c>
@@ -4600,7 +4817,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>44677</v>
       </c>
@@ -4608,7 +4825,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>44678</v>
       </c>
@@ -4616,7 +4833,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>44679</v>
       </c>
@@ -4624,7 +4841,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>44680</v>
       </c>
@@ -4632,7 +4849,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>44681</v>
       </c>
@@ -4640,7 +4857,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>44682</v>
       </c>
@@ -4648,7 +4865,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>44683</v>
       </c>
@@ -4656,7 +4873,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>44684</v>
       </c>
@@ -4664,7 +4881,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>44685</v>
       </c>
@@ -4672,7 +4889,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>44686</v>
       </c>
@@ -4680,7 +4897,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>44687</v>
       </c>
@@ -4688,7 +4905,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>44688</v>
       </c>
@@ -4696,7 +4913,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>44689</v>
       </c>
@@ -4704,7 +4921,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>44690</v>
       </c>
@@ -4712,7 +4929,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>44691</v>
       </c>
@@ -4720,7 +4937,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>44692</v>
       </c>
@@ -4728,7 +4945,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>44693</v>
       </c>
@@ -4736,7 +4953,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>44694</v>
       </c>
@@ -4744,7 +4961,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>44695</v>
       </c>
@@ -4752,7 +4969,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>44696</v>
       </c>
@@ -4760,7 +4977,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>44697</v>
       </c>
@@ -4768,7 +4985,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>44698</v>
       </c>
@@ -4776,7 +4993,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>44699</v>
       </c>
@@ -4784,7 +5001,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>44700</v>
       </c>
@@ -4792,7 +5009,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>44701</v>
       </c>
@@ -4800,7 +5017,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>44702</v>
       </c>
@@ -4808,7 +5025,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>44703</v>
       </c>
@@ -4816,7 +5033,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>44704</v>
       </c>
@@ -4824,7 +5041,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>44705</v>
       </c>
@@ -4832,7 +5049,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>44706</v>
       </c>
@@ -4840,7 +5057,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>44707</v>
       </c>
@@ -4848,7 +5065,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>44708</v>
       </c>
@@ -4856,7 +5073,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>44709</v>
       </c>
@@ -4864,7 +5081,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>44710</v>
       </c>
@@ -4872,7 +5089,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>44711</v>
       </c>
@@ -4880,7 +5097,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>44712</v>
       </c>
@@ -4888,7 +5105,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>44713</v>
       </c>
@@ -4896,7 +5113,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>44714</v>
       </c>
@@ -4904,7 +5121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>44715</v>
       </c>
@@ -4912,7 +5129,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>44716</v>
       </c>
@@ -4920,7 +5137,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>44717</v>
       </c>
@@ -4928,7 +5145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>44718</v>
       </c>
@@ -4936,7 +5153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>44719</v>
       </c>
@@ -4944,7 +5161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>44720</v>
       </c>
@@ -4952,7 +5169,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>44721</v>
       </c>
@@ -4960,7 +5177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>44722</v>
       </c>
@@ -4968,7 +5185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>44723</v>
       </c>
@@ -4976,12 +5193,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>45413</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>45414</v>
       </c>
@@ -4989,17 +5206,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>45415</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>45416</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>45417</v>
       </c>
@@ -5007,7 +5224,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>45418</v>
       </c>
@@ -5015,7 +5232,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>45419</v>
       </c>
@@ -5023,7 +5240,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>45420</v>
       </c>
@@ -5031,7 +5248,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>45421</v>
       </c>
@@ -5039,7 +5256,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>45422</v>
       </c>
@@ -5047,7 +5264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>45423</v>
       </c>
@@ -5055,7 +5272,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>45424</v>
       </c>
@@ -5063,7 +5280,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>45425</v>
       </c>
@@ -5071,7 +5288,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>45426</v>
       </c>
@@ -5079,7 +5296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>45427</v>
       </c>
@@ -5087,7 +5304,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>45428</v>
       </c>
@@ -5095,7 +5312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>45429</v>
       </c>
@@ -5103,72 +5320,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>45430</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>45431</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>45432</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>45433</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>45434</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>45435</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>45436</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>45437</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>45438</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>45439</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>45440</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>45441</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>45442</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>45443</v>
       </c>
@@ -5176,42 +5393,42 @@
         <v>82</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>45444</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>45445</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>45446</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>45447</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>45448</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>45449</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>45450</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>45451</v>
       </c>
@@ -5219,7 +5436,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>45452</v>
       </c>
@@ -5227,22 +5444,256 @@
         <v>22</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>45453</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>45454</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>45455</v>
       </c>
       <c r="B137">
         <v>12</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="4">
+        <v>45060</v>
+      </c>
+      <c r="B138">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="4">
+        <v>45061</v>
+      </c>
+      <c r="B139">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="4">
+        <v>45062</v>
+      </c>
+      <c r="B140">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="4">
+        <v>45063</v>
+      </c>
+      <c r="B141">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="4">
+        <v>45064</v>
+      </c>
+      <c r="B142">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="4">
+        <v>45065</v>
+      </c>
+      <c r="B143">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="4">
+        <v>45066</v>
+      </c>
+      <c r="B144">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="4">
+        <v>45067</v>
+      </c>
+      <c r="B145">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="4">
+        <v>45068</v>
+      </c>
+      <c r="B146">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="4">
+        <v>45069</v>
+      </c>
+      <c r="B147">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="4">
+        <v>45070</v>
+      </c>
+      <c r="B148">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="4">
+        <v>45071</v>
+      </c>
+      <c r="B149">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="4">
+        <v>45072</v>
+      </c>
+      <c r="B150">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="4">
+        <v>45073</v>
+      </c>
+      <c r="B151">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="4">
+        <v>45074</v>
+      </c>
+      <c r="B152">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="4">
+        <v>45075</v>
+      </c>
+      <c r="B153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="4">
+        <v>45076</v>
+      </c>
+      <c r="B154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="4">
+        <v>45077</v>
+      </c>
+      <c r="B155">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="4">
+        <v>45078</v>
+      </c>
+      <c r="B156">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="4">
+        <v>45079</v>
+      </c>
+      <c r="B157">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="4">
+        <v>45080</v>
+      </c>
+      <c r="B158">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="4">
+        <v>45081</v>
+      </c>
+      <c r="B159">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="4">
+        <v>45082</v>
+      </c>
+      <c r="B160">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="4">
+        <v>45083</v>
+      </c>
+      <c r="B161">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="4">
+        <v>45084</v>
+      </c>
+      <c r="B162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="4">
+        <v>45085</v>
+      </c>
+      <c r="B163">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="4">
+        <v>45086</v>
+      </c>
+      <c r="B164">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="4">
+        <v>45087</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="4">
+        <v>45088</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="4">
+        <v>45089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>